<commit_message>
Add link in readme to S2 idea. Update 3D views
</commit_message>
<xml_diff>
--- a/production/IT8951-HAT-BOM.xlsx
+++ b/production/IT8951-HAT-BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="10750" windowHeight="8030"/>
+    <workbookView activeTab="0" windowWidth="8460" windowHeight="7870"/>
   </bookViews>
   <sheets>
     <sheet name="IT8951-HAT-BOM.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7" count="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8" count="8">
   <si>
     <t>C_0805_2012Metric</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>ESP32-S3-WROOM-1-N8</t>
+  </si>
+  <si>
+    <t>AP22802AW5-7</t>
   </si>
   <si>
     <t>USB_C_Receptacle_HRO_TYPE-C-31-M-12</t>
@@ -102,18 +105,19 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A29" sqref="A29:IV29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="0" width="14.42770432692308" customWidth="1"/>
-    <col min="2" max="2" style="0" width="32.283774038461544" customWidth="1"/>
-    <col min="3" max="3" style="0" width="22.57007211538462" customWidth="1"/>
-    <col min="4" max="256" style="0" width="9.142307692307693"/>
+    <col min="1" max="1" style="0" width="17.99891826923077" customWidth="1"/>
+    <col min="2" max="2" style="0" width="16.85612980769231" customWidth="1"/>
+    <col min="3" max="3" style="0" width="28.284014423076925" customWidth="1"/>
+    <col min="4" max="4" style="0" width="13.284915865384617" customWidth="1"/>
+    <col min="5" max="256" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13.5">
@@ -519,147 +523,145 @@
     <row r="21" spans="1:4" ht="13.5">
       <c r="A21" t="inlineStr">
         <is>
-          <t>R19</t>
+          <t>U8</t>
         </is>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>560Ω</t>
-        </is>
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>C23204</t>
+          <t>C211404</t>
         </is>
       </c>
     </row>
     <row r="22" spans="1:4" ht="13.5">
       <c r="A22" t="inlineStr">
         <is>
-          <t>J8</t>
+          <t>R19</t>
         </is>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>USB_C_JTAG</t>
-        </is>
-      </c>
-      <c r="D22" t="s">
-        <v>6</v>
+          <t>560Ω</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>C23204</t>
+        </is>
       </c>
     </row>
     <row r="23" spans="1:4" ht="13.5">
       <c r="A23" t="inlineStr">
         <is>
-          <t>R9,R10</t>
+          <t>J8</t>
         </is>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>4.7K</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>C23162</t>
-        </is>
+          <t>USB_C_JTAG</t>
+        </is>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13.5">
       <c r="A24" t="inlineStr">
         <is>
-          <t>U5</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>QFN-24-1EP_4x4mm_P0.5mm_EP2.6x2.6mm</t>
-        </is>
+          <t>R9,R10</t>
+        </is>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>CP2102N-Axx-xQFN24</t>
+          <t>4.7K</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>C969913</t>
+          <t>C23162</t>
         </is>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13.5">
       <c r="A25" t="inlineStr">
         <is>
-          <t>J4</t>
-        </is>
-      </c>
-      <c r="B25" t="s">
-        <v>5</v>
+          <t>U5</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>QFN-24-1EP_4x4mm_P0.5mm_EP2.6x2.6mm</t>
+        </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>USB_C_Programming</t>
-        </is>
-      </c>
-      <c r="D25" t="s">
-        <v>6</v>
+          <t>CP2102N-Axx-xQFN24</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>C969151</t>
+        </is>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.5">
       <c r="A26" t="inlineStr">
         <is>
-          <t>SW1</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Alps_SKRK</t>
-        </is>
+          <t>J4</t>
+        </is>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>RESET</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>C202388</t>
-        </is>
+          <t>USB_C_Programming</t>
+        </is>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="13.5">
       <c r="A27" t="inlineStr">
         <is>
-          <t>R6</t>
-        </is>
-      </c>
-      <c r="B27" t="s">
-        <v>2</v>
+          <t>SW1</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Alps_SKRK</t>
+        </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>680Ω</t>
+          <t>RESET</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>C23228</t>
+          <t>C202388</t>
         </is>
       </c>
     </row>
     <row r="28" spans="1:4" ht="13.5">
       <c r="A28" t="inlineStr">
         <is>
-          <t>R2,R4</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="B28" t="s">
@@ -667,92 +669,112 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>5K</t>
+          <t>680Ω</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>C23046</t>
+          <t>C23228</t>
         </is>
       </c>
     </row>
     <row r="29" spans="1:4" ht="13.5">
       <c r="A29" t="inlineStr">
         <is>
-          <t>U4</t>
+          <t>R2,R4</t>
         </is>
       </c>
       <c r="B29" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>MCP1700-3302E_SOT23</t>
+          <t>5K</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>C39051</t>
+          <t>C23046</t>
         </is>
       </c>
     </row>
     <row r="30" spans="1:4" ht="13.5">
       <c r="A30" t="inlineStr">
         <is>
-          <t>U6</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>SOT-23-6</t>
-        </is>
+          <t>U4</t>
+        </is>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>MT3608</t>
+          <t>MCP1700-3302E_SOT23</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>C2932326</t>
+          <t>C39051</t>
         </is>
       </c>
     </row>
     <row r="31" spans="1:4" ht="13.5">
       <c r="A31" t="inlineStr">
         <is>
-          <t>R13</t>
-        </is>
-      </c>
-      <c r="B31" t="s">
-        <v>2</v>
+          <t>U6</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>SOT-23-6</t>
+        </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>442K</t>
+          <t>MT3608</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>C23175</t>
+          <t>C2932326</t>
         </is>
       </c>
     </row>
     <row r="32" spans="1:4" ht="13.5">
       <c r="A32" t="inlineStr">
         <is>
+          <t>R13</t>
+        </is>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>442K</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>C23175</t>
+        </is>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="13.5">
+      <c r="A33" t="inlineStr">
+        <is>
           <t>C9</t>
         </is>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>0</v>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>100 nF</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>C28233</t>
         </is>

</xml_diff>